<commit_message>
Added direct_load.py This script can be used to quickly run the AI program without having to learn the features or embeddings of images in the `photos` directory. It will save alot of time if you simply want to recognise a person without needing to learn all embeddings from scratch.
</commit_message>
<xml_diff>
--- a/attendance_2023-08-03.xlsx
+++ b/attendance_2023-08-03.xlsx
@@ -515,31 +515,11 @@
           <t>absent</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2023-08-03</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>02:49:19</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2023-08-03</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>02:49:26</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0:00:07</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -559,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>02:29:26</t>
+          <t>20:28:02</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -569,12 +549,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>02:29:36</t>
+          <t>20:28:08</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0:00:10</t>
+          <t>0:00:06</t>
         </is>
       </c>
     </row>

</xml_diff>